<commit_message>
Ex08_01 Recursion and DP
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milind Singh\Desktop\Programming Practice - Gits\Cracking the Coding Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75719FB-C53C-42D0-A73B-EC184CFBFB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0E78F9-E12E-4363-995B-D78E8A2F3FEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Day/Exercise</t>
   </si>
@@ -58,14 +58,67 @@
   </si>
   <si>
     <t>isPermutationPalindrome</t>
+  </si>
+  <si>
+    <t>isOneEditAway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete given Node ptr from Linked List </t>
+  </si>
+  <si>
+    <t>delete nth Node from end of list</t>
+  </si>
+  <si>
+    <t>reverse Single Linked List</t>
+  </si>
+  <si>
+    <t>recursiveReverse Single Linked List</t>
+  </si>
+  <si>
+    <t>palindrome Linked List</t>
+  </si>
+  <si>
+    <t>LC24 SwapNodes</t>
+  </si>
+  <si>
+    <t>Search In BST Recursive</t>
+  </si>
+  <si>
+    <t>Search In BST Iterative</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle Recursive</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle DP</t>
+  </si>
+  <si>
+    <t>Fibonacci Recursive DP</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>maximum depth of BST</t>
+  </si>
+  <si>
+    <t>Power of Num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,8 +146,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,135 +437,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
+        <v>44161</v>
+      </c>
+      <c r="C1" s="3">
+        <v>44162</v>
+      </c>
+      <c r="D1" s="3">
+        <v>44163</v>
+      </c>
+      <c r="E1" s="3">
+        <v>44164</v>
+      </c>
+      <c r="F1" s="3">
+        <v>44165</v>
+      </c>
+      <c r="G1" s="3">
+        <v>44166</v>
+      </c>
+      <c r="H1" s="3">
+        <v>44167</v>
+      </c>
+      <c r="I1" s="3">
+        <v>44168</v>
+      </c>
+      <c r="J1" s="3">
+        <v>44169</v>
+      </c>
+      <c r="K1" s="3">
+        <v>44170</v>
+      </c>
+      <c r="L1" s="3">
+        <v>44171</v>
+      </c>
+      <c r="M1" s="3">
+        <v>44172</v>
+      </c>
+      <c r="N1" s="3">
+        <v>44173</v>
+      </c>
+      <c r="O1" s="3">
+        <v>44174</v>
+      </c>
+      <c r="P1" s="3">
+        <v>44175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="K1">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>